<commit_message>
Adição do requisito de Imagem
</commit_message>
<xml_diff>
--- a/TG/Documentos/Requisitos.xlsx
+++ b/TG/Documentos/Requisitos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24805"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fatecspgov-my.sharepoint.com/personal/tiago_temoteo_fatec_sp_gov_br/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Documents\Projetos\Controle de estoque NS-GIO\TG_Prodam\TG\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{8426681D-3651-421F-B31B-EA227BEB9856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E9818F7-494B-4E06-921D-109E7853D29C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF7D402-0485-4E04-AD4E-93724C036084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{22304CA3-5D54-460C-AD84-D1BF7EBBC888}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Nº</t>
   </si>
@@ -254,12 +254,18 @@
   <si>
     <t>RN</t>
   </si>
+  <si>
+    <t>Manter tipo de licença</t>
+  </si>
+  <si>
+    <t>O sistema deve possibilitar que um tipo de licença seja cadastrada, alterada, excluída e consultada.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,7 +381,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -671,21 +677,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ECB6CF2-5B2A-449F-819B-BEE5D32A7EC3}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="70.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -699,7 +705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="25.5">
+    <row r="2" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
@@ -709,7 +715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="25.5">
+    <row r="3" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
@@ -719,7 +725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="25.5">
+    <row r="4" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
@@ -729,7 +735,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="25.5">
+    <row r="5" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
@@ -739,7 +745,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="25.5">
+    <row r="6" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
@@ -749,7 +755,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="25.5">
+    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3" t="s">
@@ -759,233 +765,243 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="25.5">
+    <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="25.5">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="25.5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="25.5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="2"/>
       <c r="C14" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="2"/>
       <c r="C18" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="2"/>
       <c r="C19" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="2"/>
       <c r="C20" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="25.5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="2"/>
       <c r="C21" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="25.5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="2"/>
       <c r="C22" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="25.5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="2"/>
       <c r="C23" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="25.5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="2"/>
       <c r="C24" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="25.5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="2"/>
       <c r="C26" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="65.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="2"/>
       <c r="C27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="65.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D28" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="25.5">
-      <c r="A28" s="5"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="25.5">
+    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="7"/>
       <c r="C29" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="25.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="7"/>
       <c r="C30" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1016,22 +1032,22 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>64</v>
       </c>

</xml_diff>